<commit_message>
Adding debug settings to enable the games
</commit_message>
<xml_diff>
--- a/Config/config.xlsx
+++ b/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Academic\waiting-game-DD-software\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301B024E-BBA8-4290-B542-B241617917D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12192D68-998C-4671-A987-2A3AE293DE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="5" xr2:uid="{C1A4B048-5E60-4E3A-A7F7-90BA77E30513}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
   <si>
     <t>Id</t>
   </si>
@@ -392,6 +392,15 @@
   </si>
   <si>
     <t>Always Imaginary First</t>
+  </si>
+  <si>
+    <t>Imaginary Game Enabled</t>
+  </si>
+  <si>
+    <t>Real Game Enabled</t>
+  </si>
+  <si>
+    <t>Patience Game Enabled</t>
   </si>
 </sst>
 </file>
@@ -2026,31 +2035,53 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF933835-97D0-42C7-875C-9F484192A7BE}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="b">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>58</v>
+      </c>
+      <c r="C2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>